<commit_message>
template upgrade + resolve only after complete
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Desktop/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/College/invoice-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBAD990-4C21-1A45-B1B8-0E38FF5A8131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFD9546-E9AD-C647-A32F-A1873A66DC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C17CFDA3-9E76-46FB-9DC1-21D687EE5D5D}"/>
   </bookViews>
@@ -36,59 +36,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>TAX INVOICE</t>
   </si>
   <si>
-    <t>Invoice Number</t>
-  </si>
-  <si>
     <t>%INVOICE_NUMBER%</t>
   </si>
   <si>
-    <t>Invoice Date</t>
-  </si>
-  <si>
     <t>%INVOICE_DATE%</t>
   </si>
   <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">%CUSTOMER_NAME%		</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t xml:space="preserve">%CUSTOMER_ADDRESS%		</t>
   </si>
   <si>
     <t>Statesman Bespoke</t>
   </si>
   <si>
-    <t>Montieth Road, Egmore</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>%CUSTOMER_PHONE%</t>
   </si>
   <si>
-    <t>+91 99999 99999</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>%CUSTOMER_EMAIL%</t>
   </si>
   <si>
-    <t>GSTIN: 33AEOFS0684N1ZE</t>
-  </si>
-  <si>
     <t>Item No.</t>
   </si>
   <si>
@@ -617,15 +590,9 @@
     <t>%ITEM_15_ITEM_TOTAL%</t>
   </si>
   <si>
-    <t>Amount before Tax</t>
-  </si>
-  <si>
     <t>%AMT_BEFORE_TAX%</t>
   </si>
   <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
     <t>Rs.</t>
   </si>
   <si>
@@ -638,27 +605,15 @@
     <t>%PAYMENT_METHOD%</t>
   </si>
   <si>
-    <t>Total CGST</t>
-  </si>
-  <si>
     <t>%TOTAL_CGST%</t>
   </si>
   <si>
-    <t>Total SGST</t>
-  </si>
-  <si>
     <t>%TOTAL_SGST%</t>
   </si>
   <si>
-    <t>Total IGST</t>
-  </si>
-  <si>
     <t>%TOTAL_IGST%</t>
   </si>
   <si>
-    <t>Total Tax</t>
-  </si>
-  <si>
     <t>%TOTAL_TAX%</t>
   </si>
   <si>
@@ -666,13 +621,61 @@
   </si>
   <si>
     <t>%GRAND_TOTAL%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Name: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: </t>
+  </si>
+  <si>
+    <t>%AMT_IN_WORDS%</t>
+  </si>
+  <si>
+    <t>Authorized Signature</t>
+  </si>
+  <si>
+    <t>GSTIN: 33AFCFS3119R1ZO</t>
+  </si>
+  <si>
+    <t>Invoice Number:</t>
+  </si>
+  <si>
+    <t>14/60, Sindur Eternity, Red Cross Rd, Egmore, Chennai, Tamil Nadu 600008</t>
+  </si>
+  <si>
+    <t>Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>+91 900 300 5557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Words: </t>
+  </si>
+  <si>
+    <t>Payment due in full at purchase</t>
+  </si>
+  <si>
+    <t>Cancellations: Vary for custom vs.              ready-to-wear items</t>
+  </si>
+  <si>
+    <t>Custom items: Non-returnable     /exchangeable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,6 +717,45 @@
       <name val="PalatinoLinotype-Bold-Identity-"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -735,87 +777,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -828,52 +795,99 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,213 +895,219 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,15 +1131,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>746648</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>1946868</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>173787</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>461317</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>64164</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1142,8 +1162,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1381648" y="114300"/>
-          <a:ext cx="1394941" cy="1081524"/>
+          <a:off x="2581868" y="249429"/>
+          <a:ext cx="2240713" cy="1740669"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1153,6 +1173,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1455,947 +1479,1035 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="254" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="4" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8" style="3" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" style="3" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="3.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="1"/>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="2"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="M2" s="6"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="41"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="4"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="H3" s="51" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="50" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="40"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="4"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="H4" s="50" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="41"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="40"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="41"/>
+    </row>
+    <row r="6" spans="1:13" ht="21" customHeight="1">
+      <c r="A6" s="40"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="4"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="H5" s="53" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="41"/>
+    </row>
+    <row r="7" spans="1:13" ht="15">
+      <c r="A7" s="40"/>
+      <c r="B7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="35" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="41"/>
+    </row>
+    <row r="8" spans="1:13" ht="24" customHeight="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="41"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="40"/>
+      <c r="B9" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="H6" s="55" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="41"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="40"/>
+      <c r="B10" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="39" t="s">
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="41"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="40"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="41"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="40"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="41"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="40"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="41"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" customHeight="1">
+      <c r="A14" s="40"/>
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="4"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="31" t="s">
+      <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="4"/>
-      <c r="B9" s="29" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="H9" s="34" t="s">
+      <c r="E14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="36" t="s">
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="37"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="4"/>
-      <c r="B10" s="29" t="s">
+      <c r="G14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="H10" s="34" t="s">
+      <c r="H14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="32" t="s">
+      <c r="I14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="4"/>
-      <c r="B11" s="31" t="s">
+      <c r="J14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="4"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="4"/>
-      <c r="J13" s="10"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="24">
-      <c r="A14" s="4"/>
-      <c r="B14" s="11" t="s">
+      <c r="K14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="L14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="M14" s="41"/>
+    </row>
+    <row r="15" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A15" s="40"/>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="E15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="G15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="H15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="I15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="J15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="9" t="s">
+      <c r="K15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="L15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="M15" s="41"/>
+    </row>
+    <row r="16" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A16" s="40"/>
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="F16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="G16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="H16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="25" t="s">
+      <c r="I16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="J16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="9" t="s">
+      <c r="K16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="L16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="M16" s="41"/>
+    </row>
+    <row r="17" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A17" s="40"/>
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="D17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="E17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="G17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="H17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="I17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="J17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="9" t="s">
+      <c r="K17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="L17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="M17" s="41"/>
+    </row>
+    <row r="18" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A18" s="40"/>
+      <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="D18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="E18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="F18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="G18" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="H18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="I18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="J18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="9" t="s">
+      <c r="K18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="L18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="M18" s="41"/>
+    </row>
+    <row r="19" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A19" s="40"/>
+      <c r="B19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="C19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="D19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="F19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="G19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="H19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="I19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="J19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="9" t="s">
+      <c r="K19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="L19" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="M19" s="41"/>
+    </row>
+    <row r="20" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A20" s="40"/>
+      <c r="B20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="C20" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="D20" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="E20" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="F20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="G20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="H20" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="25" t="s">
+      <c r="I20" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="J20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="9" t="s">
+      <c r="K20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="L20" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="M20" s="41"/>
+    </row>
+    <row r="21" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A21" s="40"/>
+      <c r="B21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="C21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="D21" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="E21" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="F21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="G21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="H21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K20" s="25" t="s">
+      <c r="I21" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="J21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="9" t="s">
+      <c r="K21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="L21" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="M21" s="41"/>
+    </row>
+    <row r="22" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A22" s="40"/>
+      <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="C22" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="D22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="E22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="F22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I21" s="25" t="s">
+      <c r="G22" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="H22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="I22" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="L21" s="25" t="s">
+      <c r="J22" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M21" s="6"/>
-    </row>
-    <row r="22" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="B22" s="9" t="s">
+      <c r="K22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="L22" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="M22" s="41"/>
+    </row>
+    <row r="23" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A23" s="40"/>
+      <c r="B23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="C23" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="D23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="E23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="F23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="G23" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="H23" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K22" s="25" t="s">
+      <c r="I23" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L22" s="25" t="s">
+      <c r="J23" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="9" t="s">
+      <c r="K23" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="L23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="M23" s="41"/>
+    </row>
+    <row r="24" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A24" s="40"/>
+      <c r="B24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="C24" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="D24" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="E24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="F24" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="G24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="H24" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K23" s="25" t="s">
+      <c r="I24" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="L23" s="25" t="s">
+      <c r="J24" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="M23" s="6"/>
-    </row>
-    <row r="24" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A24" s="4"/>
-      <c r="B24" s="9" t="s">
+      <c r="K24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="L24" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="M24" s="41"/>
+    </row>
+    <row r="25" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A25" s="40"/>
+      <c r="B25" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="C25" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="D25" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="E25" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="F25" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="G25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="H25" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K24" s="25" t="s">
+      <c r="I25" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L24" s="25" t="s">
+      <c r="J25" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="9" t="s">
+      <c r="K25" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="L25" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="M25" s="41"/>
+    </row>
+    <row r="26" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A26" s="40"/>
+      <c r="B26" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="C26" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="D26" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="E26" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="F26" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="G26" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="H26" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K25" s="25" t="s">
+      <c r="I26" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="L25" s="25" t="s">
+      <c r="J26" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="9" t="s">
+      <c r="K26" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="L26" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="M26" s="41"/>
+    </row>
+    <row r="27" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A27" s="40"/>
+      <c r="B27" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="C27" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="D27" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="E27" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="F27" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="G27" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="H27" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="K26" s="25" t="s">
+      <c r="I27" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="L26" s="25" t="s">
+      <c r="J27" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="9" t="s">
+      <c r="K27" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="L27" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="M27" s="41"/>
+    </row>
+    <row r="28" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A28" s="40"/>
+      <c r="B28" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="C28" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="D28" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="E28" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="F28" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="I27" s="25" t="s">
+      <c r="G28" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="H28" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="K27" s="25" t="s">
+      <c r="I28" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="L27" s="25" t="s">
+      <c r="J28" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="9" t="s">
+      <c r="K28" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="L28" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="M28" s="41"/>
+    </row>
+    <row r="29" spans="1:13" ht="23.25" customHeight="1">
+      <c r="A29" s="40"/>
+      <c r="B29" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="C29" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="D29" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="E29" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="F29" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="I28" s="25" t="s">
+      <c r="G29" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="H29" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="I29" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="L28" s="25" t="s">
+      <c r="J29" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="9" t="s">
+      <c r="K29" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="L29" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="M29" s="41"/>
+    </row>
+    <row r="30" spans="1:13" ht="24" customHeight="1">
+      <c r="A30" s="40"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="H30" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="I30" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="J30" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="K30" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="L30" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="M30" s="41"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" customHeight="1">
+      <c r="A31" s="40"/>
+      <c r="B31" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="F29" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G29" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="H29" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="I29" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="J29" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="K29" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="L29" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" ht="24" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="43" t="s">
-        <v>193</v>
-      </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="8" t="s">
+      <c r="L31" s="60" t="s">
         <v>194</v>
       </c>
-      <c r="I30" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="J30" s="35"/>
-      <c r="K30" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="L30" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="M30" s="6"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="4"/>
-      <c r="B31" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32" t="s">
+      <c r="M31" s="41"/>
+    </row>
+    <row r="32" spans="1:13" ht="11" customHeight="1">
+      <c r="A32" s="40"/>
+      <c r="B32" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="I32" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" s="4"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="5"/>
-      <c r="I32" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="L32" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="M32" s="6"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="57"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="41"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="4"/>
-      <c r="I33" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="J33" s="33"/>
-      <c r="K33" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="L33" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="M33" s="6"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="61" t="s">
+        <v>208</v>
+      </c>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="41"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="4"/>
-      <c r="I34" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="J34" s="33"/>
-      <c r="K34" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="L34" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="M34" s="6"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="41"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="4"/>
-      <c r="I35" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="J35" s="33"/>
-      <c r="K35" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="L35" s="15" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="41"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="40"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="67" t="s">
         <v>209</v>
       </c>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="4"/>
-      <c r="M36" s="6"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="4"/>
-      <c r="M37" s="6"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="41"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="18"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="21"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="B2:F7"/>
+  <mergeCells count="27">
+    <mergeCell ref="D36:G37"/>
+    <mergeCell ref="D34:G35"/>
+    <mergeCell ref="B33:C37"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I32:L34"/>
+    <mergeCell ref="D33:G33"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I8"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="J6:L8"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J3:L3"/>
@@ -2406,18 +2518,9 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="E31:H31"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
plsss let this be final
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/College/invoice-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA93B980-44CC-0E40-AF8C-DF94AAAC3EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CA80D45-6847-854E-B585-EA2A86AF838F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C17CFDA3-9E76-46FB-9DC1-21D687EE5D5D}"/>
   </bookViews>
@@ -1036,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1095,24 +1095,69 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1173,58 +1218,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1593,7 +1602,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="182" zoomScaleNormal="254" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11"/>
@@ -1616,19 +1625,19 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1">
@@ -1638,11 +1647,11 @@
     <row r="3" spans="1:13" ht="11" customHeight="1">
       <c r="A3" s="4"/>
       <c r="C3" s="22"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" ht="11" customHeight="1">
@@ -1651,45 +1660,45 @@
         <v>205</v>
       </c>
       <c r="C4" s="22"/>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="53" t="s">
+      <c r="I4" s="40"/>
+      <c r="J4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
       <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="23" customHeight="1">
       <c r="A5" s="4"/>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="H5" s="26" t="s">
+      <c r="C5" s="37"/>
+      <c r="H5" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="64" t="s">
+      <c r="I5" s="41"/>
+      <c r="J5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" ht="14" customHeight="1">
       <c r="A6" s="4"/>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="64" t="s">
+      <c r="I6" s="41"/>
+      <c r="J6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
       <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="15">
@@ -1698,27 +1707,27 @@
         <v>5</v>
       </c>
       <c r="C7" s="20"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="24" customHeight="1">
       <c r="A8" s="4"/>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="27"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:13">
@@ -1726,15 +1735,15 @@
       <c r="B9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="61" t="s">
+      <c r="I9" s="41"/>
+      <c r="J9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="22" customHeight="1">
@@ -1743,28 +1752,28 @@
         <v>204</v>
       </c>
       <c r="C10" s="19"/>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="I10" s="52"/>
-      <c r="J10" s="62" t="s">
+      <c r="I10" s="35"/>
+      <c r="J10" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4"/>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53" t="s">
+      <c r="I11" s="35"/>
+      <c r="J11" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
       <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13">
@@ -2395,21 +2404,21 @@
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" s="4"/>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="41" t="s">
+      <c r="C31" s="29"/>
+      <c r="D31" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="69" t="s">
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
       <c r="K31" s="21" t="s">
         <v>186</v>
       </c>
@@ -2420,96 +2429,96 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="4"/>
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="38" t="s">
+      <c r="C32" s="31"/>
+      <c r="D32" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="66" t="s">
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="67" t="s">
         <v>202</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="29"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="69"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="4"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="49" t="s">
+      <c r="B33" s="47"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="31"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="44"/>
       <c r="M33" s="5"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="4"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="43" t="s">
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="45"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="60"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
       <c r="K34" s="15"/>
       <c r="L34" s="16"/>
       <c r="M34" s="5"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="4"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="45"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
       <c r="M35" s="5"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="4"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="43" t="s">
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="45"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
       <c r="M36" s="5"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="4"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="63"/>
       <c r="M37" s="5"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="7"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -2523,6 +2532,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H6:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I32:L33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="B33:C37"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D34:G35"/>
+    <mergeCell ref="D36:G37"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -2539,19 +2561,6 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I32:L33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="B33:C37"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D34:G35"/>
-    <mergeCell ref="D36:G37"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>